<commit_message>
update responsible_parties in ocn and toplevel forc cm2-sr5
</commit_message>
<xml_diff>
--- a/cmip6/models/cmcc-cm2-sr5/cmip6_cmcc_cmcc-cm2-sr5_ocean.xlsx
+++ b/cmip6/models/cmcc-cm2-sr5/cmip6_cmcc_cmcc-cm2-sr5_ocean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/ES-DOC-INST-cmcc/cmip6/models/cmcc-cm2-sr5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF571DEF-5783-B242-8577-A4F4CE670F6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B594A5-CC96-304D-83F1-0C7ADE909CA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="855">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -2588,6 +2588,18 @@
   </si>
   <si>
     <t>Blend of different dataset as described in mathiot_2007</t>
+  </si>
+  <si>
+    <t>LOVATO-TOMAS</t>
+  </si>
+  <si>
+    <t>Principal Investigator</t>
+  </si>
+  <si>
+    <t>Contributor</t>
+  </si>
+  <si>
+    <t>FOGLI-PIER-GIUSEPPE</t>
   </si>
 </sst>
 </file>
@@ -3895,10 +3907,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3943,45 +3955,49 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-    </row>
-    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+    <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>851</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>854</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="9"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B17" s="10" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
-        <v>846</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>843</v>
+        <v>846</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>40</v>
@@ -3989,7 +4005,7 @@
     </row>
     <row r="19" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>40</v>
@@ -3997,7 +4013,7 @@
     </row>
     <row r="20" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>40</v>
@@ -4005,24 +4021,32 @@
     </row>
     <row r="21" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
+        <v>848</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
         <v>844</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B22" s="11" t="s">
         <v>722</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B10" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Author,Contributor,Principal Investigator,Point of Contact,Sponsor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17:B21" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B22" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Top Level,Key Properties,Grid,Timestepping Framework,Advection,Lateral Physics,Vertical Physics,Uplow Boundaries,Boundary Forcing"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A13" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A14" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update responsible_parties in ocn
</commit_message>
<xml_diff>
--- a/cmip6/models/cmcc-cm2-sr5/cmip6_cmcc_cmcc-cm2-sr5_ocean.xlsx
+++ b/cmip6/models/cmcc-cm2-sr5/cmip6_cmcc_cmcc-cm2-sr5_ocean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/ES-DOC-INST-cmcc/cmip6/models/cmcc-cm2-sr5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B594A5-CC96-304D-83F1-0C7ADE909CA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8C53A4-5820-C04D-88E6-731AC8A6BB18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3910,7 +3910,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>